<commit_message>
Updated Timings for 3 Slides + Added Instructions html
</commit_message>
<xml_diff>
--- a/Timings.xlsx
+++ b/Timings.xlsx
@@ -52,7 +52,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -192,34 +192,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -539,7 +539,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,8 +706,14 @@
       <c r="D11" s="10"/>
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="20"/>
+      <c r="G11" s="19">
+        <f>4000/60</f>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="H11" s="20">
+        <f>G11-G10</f>
+        <v>20.000000000000007</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C12" s="2">

</xml_diff>